<commit_message>
BLE Module Finished - Passed all Important Design Rules
</commit_message>
<xml_diff>
--- a/Steering/Hardware/BOM/Steering_Controller_1R1_BOM.xlsx
+++ b/Steering/Hardware/BOM/Steering_Controller_1R1_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\files.auckland.ac.nz\myhome\Desktop\Electeng\2020-srw-rc-car\Steering\Hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF3FCB3-48B7-41EB-80F0-6817276E5C90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1BBFA6-E70E-40BF-8B39-EDF14F8CF1DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" xr2:uid="{4895F57E-8DCF-4A6C-9607-D9B5352DA2F2}"/>
   </bookViews>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14A6EB3-AA55-40DD-86B5-47847CF9DC22}">
   <dimension ref="B2:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>